<commit_message>
DAQ period must be integer microsec
</commit_message>
<xml_diff>
--- a/mcu_source/v0.2.0_VSCODE/faster_mulmod_ideas.xlsx
+++ b/mcu_source/v0.2.0_VSCODE/faster_mulmod_ideas.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vangi\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Work\_GitHub_repo\DvG_Arduino_lock-in_amp\mcu_source\v0.2.0_VSCODE\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2258955-7255-416C-AB26-F94DE17850BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CEF9B07-CE5B-4CCB-B279-E8AE6C951379}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="23000" windowHeight="14620" xr2:uid="{80EF1C06-4846-4713-BE74-B3A66229754E}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="33">
   <si>
     <t>ref_freq</t>
   </si>
@@ -123,13 +123,16 @@
     <t>BLOCK_SIZE for 10 blocks/s</t>
   </si>
   <si>
-    <t>also power of 2 ish</t>
-  </si>
-  <si>
     <t>&lt;-----</t>
   </si>
   <si>
     <t>rounded integer idx/iter</t>
+  </si>
+  <si>
+    <t>also power of 2 ish: CAN'T see period</t>
+  </si>
+  <si>
+    <t>must be int</t>
   </si>
 </sst>
 </file>
@@ -161,7 +164,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -180,6 +183,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -193,7 +202,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -235,6 +244,9 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" quotePrefix="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="2" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -552,7 +564,7 @@
   <dimension ref="A1:R61"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L15" sqref="L15"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -576,7 +588,7 @@
       </c>
       <c r="C1" s="21">
         <f>C3/10</f>
-        <v>1024</v>
+        <v>1000</v>
       </c>
       <c r="D1" s="4" t="s">
         <v>27</v>
@@ -592,7 +604,7 @@
       </c>
       <c r="J2" s="14">
         <f>J3/D6*C3</f>
-        <v>250</v>
+        <v>249.93896484375</v>
       </c>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.35">
@@ -600,24 +612,26 @@
         <v>4</v>
       </c>
       <c r="C3" s="1">
-        <v>10240</v>
+        <v>10000</v>
       </c>
       <c r="D3" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="E3" t="s">
-        <v>29</v>
-      </c>
+      <c r="E3" s="25" t="s">
+        <v>31</v>
+      </c>
+      <c r="F3" s="26"/>
+      <c r="G3" s="25"/>
       <c r="H3" s="17"/>
       <c r="I3" s="18" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="J3" s="15">
         <f>ROUND(J4,0)</f>
-        <v>800</v>
+        <v>819</v>
       </c>
       <c r="K3" s="24" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.35">
@@ -626,15 +640,22 @@
       </c>
       <c r="C4" s="20">
         <f>1/C3</f>
-        <v>9.7656250000000005E-5</v>
+        <v>1E-4</v>
       </c>
       <c r="D4" s="7" t="s">
         <v>9</v>
+      </c>
+      <c r="E4" s="27">
+        <f>C4*1000000</f>
+        <v>100</v>
+      </c>
+      <c r="F4" s="26" t="s">
+        <v>32</v>
       </c>
       <c r="H4" s="2"/>
       <c r="J4" s="16">
         <f>D6/C3*C5</f>
-        <v>800</v>
+        <v>819.2</v>
       </c>
       <c r="L4" s="22"/>
     </row>
@@ -720,7 +741,7 @@
     <row r="10" spans="1:18" x14ac:dyDescent="0.35">
       <c r="O10" s="13">
         <f>10000000/J4</f>
-        <v>12500</v>
+        <v>12207.03125</v>
       </c>
       <c r="P10" t="s">
         <v>20</v>
@@ -798,11 +819,11 @@
         <v>0</v>
       </c>
       <c r="J14" s="3">
-        <f>MOD(I14,$D$6)</f>
+        <f t="shared" ref="J14:J39" si="1">MOD(I14,$D$6)</f>
         <v>0</v>
       </c>
       <c r="K14" s="2">
-        <f>J14/($D$6)</f>
+        <f t="shared" ref="K14:K39" si="2">J14/($D$6)</f>
         <v>0</v>
       </c>
       <c r="L14">
@@ -815,7 +836,7 @@
       </c>
       <c r="O14" s="13">
         <f>POWER(2,32)/J4</f>
-        <v>5368709.1200000001</v>
+        <v>5242880</v>
       </c>
       <c r="P14" t="s">
         <v>20</v>
@@ -826,39 +847,39 @@
         <v>1</v>
       </c>
       <c r="B15" s="6">
-        <f t="shared" ref="B15:B39" si="1">A15*1/$C$3*1000</f>
-        <v>9.765625E-2</v>
+        <f t="shared" ref="B15:B39" si="3">A15*1/$C$3*1000</f>
+        <v>0.1</v>
       </c>
       <c r="E15" s="2">
-        <f t="shared" ref="E15:E39" si="2">$C$5*B15/1000</f>
-        <v>2.44140625E-2</v>
+        <f t="shared" ref="E15:E39" si="4">$C$5*B15/1000</f>
+        <v>2.5000000000000001E-2</v>
       </c>
       <c r="F15" s="8">
         <f t="shared" si="0"/>
-        <v>0.15279718525844341</v>
+        <v>0.15643446504023087</v>
       </c>
       <c r="H15" s="2">
-        <f t="shared" ref="H15:H39" si="3">$J$4*A15</f>
-        <v>800</v>
+        <f t="shared" ref="H15:H39" si="5">$J$4*A15</f>
+        <v>819.2</v>
       </c>
       <c r="I15" s="3">
-        <f t="shared" ref="I15:I61" si="4">ROUND(H15,0)</f>
-        <v>800</v>
+        <f t="shared" ref="I15:I61" si="6">ROUND(H15,0)</f>
+        <v>819</v>
       </c>
       <c r="J15" s="3">
-        <f>MOD(I15,$D$6)</f>
-        <v>800</v>
+        <f t="shared" si="1"/>
+        <v>819</v>
       </c>
       <c r="K15" s="2">
-        <f>J15/($D$6)</f>
-        <v>2.44140625E-2</v>
+        <f t="shared" si="2"/>
+        <v>2.4993896484375E-2</v>
       </c>
       <c r="L15">
-        <f t="shared" ref="L15:L39" si="5">_xlfn.BITAND(I15,$D$6-1)</f>
-        <v>800</v>
+        <f t="shared" ref="L15:L39" si="7">_xlfn.BITAND(I15,$D$6-1)</f>
+        <v>819</v>
       </c>
       <c r="M15" s="2">
-        <f t="shared" ref="M15:M39" si="6">$L$4*B15/1000</f>
+        <f t="shared" ref="M15:M39" si="8">$L$4*B15/1000</f>
         <v>0</v>
       </c>
       <c r="O15" s="13">
@@ -874,39 +895,39 @@
         <v>2</v>
       </c>
       <c r="B16" s="6">
-        <f t="shared" si="1"/>
-        <v>0.1953125</v>
+        <f t="shared" si="3"/>
+        <v>0.2</v>
       </c>
       <c r="E16" s="2">
-        <f t="shared" si="2"/>
-        <v>4.8828125E-2</v>
+        <f t="shared" si="4"/>
+        <v>0.05</v>
       </c>
       <c r="F16" s="8">
         <f t="shared" si="0"/>
-        <v>0.30200594931922803</v>
+        <v>0.3090169943749474</v>
       </c>
       <c r="H16" s="2">
-        <f t="shared" si="3"/>
-        <v>1600</v>
+        <f t="shared" si="5"/>
+        <v>1638.4</v>
       </c>
       <c r="I16" s="3">
-        <f t="shared" si="4"/>
-        <v>1600</v>
+        <f t="shared" si="6"/>
+        <v>1638</v>
       </c>
       <c r="J16" s="3">
-        <f>MOD(I16,$D$6)</f>
-        <v>1600</v>
+        <f t="shared" si="1"/>
+        <v>1638</v>
       </c>
       <c r="K16" s="2">
-        <f>J16/($D$6)</f>
-        <v>4.8828125E-2</v>
+        <f t="shared" si="2"/>
+        <v>4.998779296875E-2</v>
       </c>
       <c r="L16">
-        <f t="shared" si="5"/>
-        <v>1600</v>
+        <f t="shared" si="7"/>
+        <v>1638</v>
       </c>
       <c r="M16" s="2">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
     </row>
@@ -915,39 +936,39 @@
         <v>3</v>
       </c>
       <c r="B17" s="6">
-        <f t="shared" si="1"/>
-        <v>0.29296875</v>
+        <f t="shared" si="3"/>
+        <v>0.3</v>
       </c>
       <c r="E17" s="2">
-        <f t="shared" si="2"/>
-        <v>7.32421875E-2</v>
+        <f t="shared" si="4"/>
+        <v>7.4999999999999997E-2</v>
       </c>
       <c r="F17" s="8">
         <f t="shared" si="0"/>
-        <v>0.4441221445704292</v>
+        <v>0.45399049973954675</v>
       </c>
       <c r="H17" s="2">
-        <f t="shared" si="3"/>
-        <v>2400</v>
+        <f t="shared" si="5"/>
+        <v>2457.6000000000004</v>
       </c>
       <c r="I17" s="3">
-        <f t="shared" si="4"/>
-        <v>2400</v>
+        <f t="shared" si="6"/>
+        <v>2458</v>
       </c>
       <c r="J17" s="3">
-        <f>MOD(I17,$D$6)</f>
-        <v>2400</v>
+        <f t="shared" si="1"/>
+        <v>2458</v>
       </c>
       <c r="K17" s="2">
-        <f>J17/($D$6)</f>
-        <v>7.32421875E-2</v>
+        <f t="shared" si="2"/>
+        <v>7.501220703125E-2</v>
       </c>
       <c r="L17">
-        <f t="shared" si="5"/>
-        <v>2400</v>
+        <f t="shared" si="7"/>
+        <v>2458</v>
       </c>
       <c r="M17" s="2">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
     </row>
@@ -956,39 +977,39 @@
         <v>4</v>
       </c>
       <c r="B18" s="6">
-        <f t="shared" si="1"/>
-        <v>0.390625</v>
+        <f t="shared" si="3"/>
+        <v>0.4</v>
       </c>
       <c r="E18" s="2">
-        <f t="shared" si="2"/>
-        <v>9.765625E-2</v>
+        <f t="shared" si="4"/>
+        <v>0.1</v>
       </c>
       <c r="F18" s="8">
         <f t="shared" si="0"/>
-        <v>0.57580819141784523</v>
+        <v>0.58778525229247314</v>
       </c>
       <c r="H18" s="2">
-        <f t="shared" si="3"/>
-        <v>3200</v>
+        <f t="shared" si="5"/>
+        <v>3276.8</v>
       </c>
       <c r="I18" s="3">
-        <f t="shared" si="4"/>
-        <v>3200</v>
+        <f t="shared" si="6"/>
+        <v>3277</v>
       </c>
       <c r="J18" s="3">
-        <f>MOD(I18,$D$6)</f>
-        <v>3200</v>
+        <f t="shared" si="1"/>
+        <v>3277</v>
       </c>
       <c r="K18" s="2">
-        <f>J18/($D$6)</f>
-        <v>9.765625E-2</v>
+        <f t="shared" si="2"/>
+        <v>0.100006103515625</v>
       </c>
       <c r="L18">
-        <f t="shared" si="5"/>
-        <v>3200</v>
+        <f t="shared" si="7"/>
+        <v>3277</v>
       </c>
       <c r="M18" s="2">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
     </row>
@@ -997,39 +1018,39 @@
         <v>5</v>
       </c>
       <c r="B19" s="6">
-        <f t="shared" si="1"/>
-        <v>0.48828125</v>
+        <f t="shared" si="3"/>
+        <v>0.5</v>
       </c>
       <c r="E19" s="2">
-        <f t="shared" si="2"/>
-        <v>0.1220703125</v>
+        <f t="shared" si="4"/>
+        <v>0.125</v>
       </c>
       <c r="F19" s="8">
         <f t="shared" si="0"/>
-        <v>0.693971460889654</v>
+        <v>0.70710678118654746</v>
       </c>
       <c r="H19" s="2">
-        <f t="shared" si="3"/>
-        <v>4000</v>
+        <f t="shared" si="5"/>
+        <v>4096</v>
       </c>
       <c r="I19" s="3">
-        <f t="shared" si="4"/>
-        <v>4000</v>
+        <f t="shared" si="6"/>
+        <v>4096</v>
       </c>
       <c r="J19" s="3">
-        <f>MOD(I19,$D$6)</f>
-        <v>4000</v>
+        <f t="shared" si="1"/>
+        <v>4096</v>
       </c>
       <c r="K19" s="2">
-        <f>J19/($D$6)</f>
-        <v>0.1220703125</v>
+        <f t="shared" si="2"/>
+        <v>0.125</v>
       </c>
       <c r="L19">
-        <f t="shared" si="5"/>
-        <v>4000</v>
+        <f t="shared" si="7"/>
+        <v>4096</v>
       </c>
       <c r="M19" s="2">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
     </row>
@@ -1038,39 +1059,39 @@
         <v>6</v>
       </c>
       <c r="B20" s="6">
-        <f t="shared" si="1"/>
-        <v>0.5859375</v>
+        <f t="shared" si="3"/>
+        <v>0.6</v>
       </c>
       <c r="E20" s="2">
-        <f t="shared" si="2"/>
-        <v>0.146484375</v>
+        <f t="shared" si="4"/>
+        <v>0.15</v>
       </c>
       <c r="F20" s="8">
         <f t="shared" si="0"/>
-        <v>0.79583690460888346</v>
+        <v>0.80901699437494734</v>
       </c>
       <c r="H20" s="2">
-        <f t="shared" si="3"/>
-        <v>4800</v>
+        <f t="shared" si="5"/>
+        <v>4915.2000000000007</v>
       </c>
       <c r="I20" s="3">
-        <f t="shared" si="4"/>
-        <v>4800</v>
+        <f t="shared" si="6"/>
+        <v>4915</v>
       </c>
       <c r="J20" s="3">
-        <f>MOD(I20,$D$6)</f>
-        <v>4800</v>
+        <f t="shared" si="1"/>
+        <v>4915</v>
       </c>
       <c r="K20" s="2">
-        <f>J20/($D$6)</f>
-        <v>0.146484375</v>
+        <f t="shared" si="2"/>
+        <v>0.149993896484375</v>
       </c>
       <c r="L20">
-        <f t="shared" si="5"/>
-        <v>4800</v>
+        <f t="shared" si="7"/>
+        <v>4915</v>
       </c>
       <c r="M20" s="2">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
     </row>
@@ -1079,39 +1100,39 @@
         <v>7</v>
       </c>
       <c r="B21" s="6">
-        <f t="shared" si="1"/>
-        <v>0.68359375</v>
+        <f t="shared" si="3"/>
+        <v>0.7</v>
       </c>
       <c r="E21" s="2">
-        <f t="shared" si="2"/>
-        <v>0.1708984375</v>
+        <f t="shared" si="4"/>
+        <v>0.17499999999999999</v>
       </c>
       <c r="F21" s="8">
         <f t="shared" si="0"/>
-        <v>0.87901222642863341</v>
+        <v>0.89100652418836779</v>
       </c>
       <c r="H21" s="2">
-        <f t="shared" si="3"/>
-        <v>5600</v>
+        <f t="shared" si="5"/>
+        <v>5734.4000000000005</v>
       </c>
       <c r="I21" s="3">
-        <f t="shared" si="4"/>
-        <v>5600</v>
+        <f t="shared" si="6"/>
+        <v>5734</v>
       </c>
       <c r="J21" s="3">
-        <f>MOD(I21,$D$6)</f>
-        <v>5600</v>
+        <f t="shared" si="1"/>
+        <v>5734</v>
       </c>
       <c r="K21" s="2">
-        <f>J21/($D$6)</f>
-        <v>0.1708984375</v>
+        <f t="shared" si="2"/>
+        <v>0.17498779296875</v>
       </c>
       <c r="L21">
-        <f t="shared" si="5"/>
-        <v>5600</v>
+        <f t="shared" si="7"/>
+        <v>5734</v>
       </c>
       <c r="M21" s="2">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
     </row>
@@ -1120,39 +1141,39 @@
         <v>8</v>
       </c>
       <c r="B22" s="6">
-        <f t="shared" si="1"/>
-        <v>0.78125</v>
+        <f t="shared" si="3"/>
+        <v>0.8</v>
       </c>
       <c r="E22" s="2">
-        <f t="shared" si="2"/>
-        <v>0.1953125</v>
+        <f t="shared" si="4"/>
+        <v>0.2</v>
       </c>
       <c r="F22" s="8">
         <f t="shared" si="0"/>
-        <v>0.9415440651830207</v>
+        <v>0.95105651629515353</v>
       </c>
       <c r="H22" s="2">
-        <f t="shared" si="3"/>
-        <v>6400</v>
+        <f t="shared" si="5"/>
+        <v>6553.6</v>
       </c>
       <c r="I22" s="3">
-        <f t="shared" si="4"/>
-        <v>6400</v>
+        <f t="shared" si="6"/>
+        <v>6554</v>
       </c>
       <c r="J22" s="3">
-        <f>MOD(I22,$D$6)</f>
-        <v>6400</v>
+        <f t="shared" si="1"/>
+        <v>6554</v>
       </c>
       <c r="K22" s="2">
-        <f>J22/($D$6)</f>
-        <v>0.1953125</v>
+        <f t="shared" si="2"/>
+        <v>0.20001220703125</v>
       </c>
       <c r="L22">
-        <f t="shared" si="5"/>
-        <v>6400</v>
+        <f t="shared" si="7"/>
+        <v>6554</v>
       </c>
       <c r="M22" s="2">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
     </row>
@@ -1161,39 +1182,39 @@
         <v>9</v>
       </c>
       <c r="B23" s="6">
-        <f t="shared" si="1"/>
-        <v>0.87890625</v>
+        <f t="shared" si="3"/>
+        <v>0.9</v>
       </c>
       <c r="E23" s="2">
-        <f t="shared" si="2"/>
-        <v>0.2197265625</v>
+        <f t="shared" si="4"/>
+        <v>0.22500000000000001</v>
       </c>
       <c r="F23" s="8">
         <f t="shared" si="0"/>
-        <v>0.98196386910955524</v>
+        <v>0.98768834059513777</v>
       </c>
       <c r="H23" s="2">
-        <f t="shared" si="3"/>
-        <v>7200</v>
+        <f t="shared" si="5"/>
+        <v>7372.8</v>
       </c>
       <c r="I23" s="3">
-        <f t="shared" si="4"/>
-        <v>7200</v>
+        <f t="shared" si="6"/>
+        <v>7373</v>
       </c>
       <c r="J23" s="3">
-        <f>MOD(I23,$D$6)</f>
-        <v>7200</v>
+        <f t="shared" si="1"/>
+        <v>7373</v>
       </c>
       <c r="K23" s="2">
-        <f>J23/($D$6)</f>
-        <v>0.2197265625</v>
+        <f t="shared" si="2"/>
+        <v>0.225006103515625</v>
       </c>
       <c r="L23">
-        <f t="shared" si="5"/>
-        <v>7200</v>
+        <f t="shared" si="7"/>
+        <v>7373</v>
       </c>
       <c r="M23" s="2">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
     </row>
@@ -1202,39 +1223,39 @@
         <v>10</v>
       </c>
       <c r="B24" s="6">
-        <f t="shared" si="1"/>
-        <v>0.9765625</v>
+        <f t="shared" si="3"/>
+        <v>1</v>
       </c>
       <c r="E24" s="2">
-        <f t="shared" si="2"/>
-        <v>0.244140625</v>
+        <f t="shared" si="4"/>
+        <v>0.25</v>
       </c>
       <c r="F24" s="8">
         <f t="shared" si="0"/>
-        <v>0.99932238458834954</v>
+        <v>1</v>
       </c>
       <c r="H24" s="2">
-        <f t="shared" si="3"/>
-        <v>8000</v>
+        <f t="shared" si="5"/>
+        <v>8192</v>
       </c>
       <c r="I24" s="3">
-        <f t="shared" si="4"/>
-        <v>8000</v>
+        <f t="shared" si="6"/>
+        <v>8192</v>
       </c>
       <c r="J24" s="3">
-        <f>MOD(I24,$D$6)</f>
-        <v>8000</v>
+        <f t="shared" si="1"/>
+        <v>8192</v>
       </c>
       <c r="K24" s="2">
-        <f>J24/($D$6)</f>
-        <v>0.244140625</v>
+        <f t="shared" si="2"/>
+        <v>0.25</v>
       </c>
       <c r="L24">
-        <f t="shared" si="5"/>
-        <v>8000</v>
+        <f t="shared" si="7"/>
+        <v>8192</v>
       </c>
       <c r="M24" s="2">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
     </row>
@@ -1243,39 +1264,39 @@
         <v>11</v>
       </c>
       <c r="B25" s="6">
-        <f t="shared" si="1"/>
-        <v>1.07421875</v>
+        <f t="shared" si="3"/>
+        <v>1.1000000000000001</v>
       </c>
       <c r="E25" s="2">
-        <f t="shared" si="2"/>
-        <v>0.2685546875</v>
+        <f t="shared" si="4"/>
+        <v>0.27500000000000002</v>
       </c>
       <c r="F25" s="8">
         <f t="shared" si="0"/>
-        <v>0.9932119492347945</v>
+        <v>0.98768834059513777</v>
       </c>
       <c r="H25" s="2">
-        <f t="shared" si="3"/>
-        <v>8800</v>
+        <f t="shared" si="5"/>
+        <v>9011.2000000000007</v>
       </c>
       <c r="I25" s="3">
-        <f t="shared" si="4"/>
-        <v>8800</v>
+        <f t="shared" si="6"/>
+        <v>9011</v>
       </c>
       <c r="J25" s="3">
-        <f>MOD(I25,$D$6)</f>
-        <v>8800</v>
+        <f t="shared" si="1"/>
+        <v>9011</v>
       </c>
       <c r="K25" s="2">
-        <f>J25/($D$6)</f>
-        <v>0.2685546875</v>
+        <f t="shared" si="2"/>
+        <v>0.274993896484375</v>
       </c>
       <c r="L25">
-        <f t="shared" si="5"/>
-        <v>8800</v>
+        <f t="shared" si="7"/>
+        <v>9011</v>
       </c>
       <c r="M25" s="2">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
     </row>
@@ -1284,39 +1305,39 @@
         <v>12</v>
       </c>
       <c r="B26" s="6">
-        <f t="shared" si="1"/>
-        <v>1.171875</v>
+        <f t="shared" si="3"/>
+        <v>1.2</v>
       </c>
       <c r="E26" s="2">
-        <f t="shared" si="2"/>
-        <v>0.29296875</v>
+        <f t="shared" si="4"/>
+        <v>0.3</v>
       </c>
       <c r="F26" s="8">
         <f t="shared" si="0"/>
-        <v>0.96377606579543984</v>
+        <v>0.95105651629515364</v>
       </c>
       <c r="H26" s="2">
-        <f t="shared" si="3"/>
-        <v>9600</v>
+        <f t="shared" si="5"/>
+        <v>9830.4000000000015</v>
       </c>
       <c r="I26" s="3">
-        <f t="shared" si="4"/>
-        <v>9600</v>
+        <f t="shared" si="6"/>
+        <v>9830</v>
       </c>
       <c r="J26" s="3">
-        <f>MOD(I26,$D$6)</f>
-        <v>9600</v>
+        <f t="shared" si="1"/>
+        <v>9830</v>
       </c>
       <c r="K26" s="2">
-        <f>J26/($D$6)</f>
-        <v>0.29296875</v>
+        <f t="shared" si="2"/>
+        <v>0.29998779296875</v>
       </c>
       <c r="L26">
-        <f t="shared" si="5"/>
-        <v>9600</v>
+        <f t="shared" si="7"/>
+        <v>9830</v>
       </c>
       <c r="M26" s="2">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
     </row>
@@ -1325,39 +1346,39 @@
         <v>13</v>
       </c>
       <c r="B27" s="6">
-        <f t="shared" si="1"/>
-        <v>1.26953125</v>
+        <f t="shared" si="3"/>
+        <v>1.3</v>
       </c>
       <c r="E27" s="2">
-        <f t="shared" si="2"/>
-        <v>0.3173828125</v>
+        <f t="shared" si="4"/>
+        <v>0.32500000000000001</v>
       </c>
       <c r="F27" s="8">
         <f t="shared" si="0"/>
-        <v>0.91170603200542999</v>
+        <v>0.8910065241883679</v>
       </c>
       <c r="H27" s="2">
-        <f t="shared" si="3"/>
-        <v>10400</v>
+        <f t="shared" si="5"/>
+        <v>10649.6</v>
       </c>
       <c r="I27" s="3">
-        <f t="shared" si="4"/>
-        <v>10400</v>
+        <f t="shared" si="6"/>
+        <v>10650</v>
       </c>
       <c r="J27" s="3">
-        <f>MOD(I27,$D$6)</f>
-        <v>10400</v>
+        <f t="shared" si="1"/>
+        <v>10650</v>
       </c>
       <c r="K27" s="2">
-        <f>J27/($D$6)</f>
-        <v>0.3173828125</v>
+        <f t="shared" si="2"/>
+        <v>0.32501220703125</v>
       </c>
       <c r="L27">
-        <f t="shared" si="5"/>
-        <v>10400</v>
+        <f t="shared" si="7"/>
+        <v>10650</v>
       </c>
       <c r="M27" s="2">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
     </row>
@@ -1366,39 +1387,39 @@
         <v>14</v>
       </c>
       <c r="B28" s="6">
-        <f t="shared" si="1"/>
-        <v>1.3671875</v>
+        <f t="shared" si="3"/>
+        <v>1.4</v>
       </c>
       <c r="E28" s="2">
-        <f t="shared" si="2"/>
-        <v>0.341796875</v>
+        <f t="shared" si="4"/>
+        <v>0.35</v>
       </c>
       <c r="F28" s="8">
         <f t="shared" si="0"/>
-        <v>0.83822470555483819</v>
+        <v>0.80901699437494745</v>
       </c>
       <c r="H28" s="2">
-        <f t="shared" si="3"/>
-        <v>11200</v>
+        <f t="shared" si="5"/>
+        <v>11468.800000000001</v>
       </c>
       <c r="I28" s="3">
-        <f t="shared" si="4"/>
-        <v>11200</v>
+        <f t="shared" si="6"/>
+        <v>11469</v>
       </c>
       <c r="J28" s="3">
-        <f>MOD(I28,$D$6)</f>
-        <v>11200</v>
+        <f t="shared" si="1"/>
+        <v>11469</v>
       </c>
       <c r="K28" s="2">
-        <f>J28/($D$6)</f>
-        <v>0.341796875</v>
+        <f t="shared" si="2"/>
+        <v>0.350006103515625</v>
       </c>
       <c r="L28">
-        <f t="shared" si="5"/>
-        <v>11200</v>
+        <f t="shared" si="7"/>
+        <v>11469</v>
       </c>
       <c r="M28" s="2">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
     </row>
@@ -1407,39 +1428,39 @@
         <v>15</v>
       </c>
       <c r="B29" s="6">
-        <f t="shared" si="1"/>
-        <v>1.46484375</v>
+        <f t="shared" si="3"/>
+        <v>1.5</v>
       </c>
       <c r="E29" s="2">
-        <f t="shared" si="2"/>
-        <v>0.3662109375</v>
+        <f t="shared" si="4"/>
+        <v>0.375</v>
       </c>
       <c r="F29" s="8">
         <f t="shared" si="0"/>
-        <v>0.74505778544146606</v>
+        <v>0.70710678118654757</v>
       </c>
       <c r="H29" s="2">
-        <f t="shared" si="3"/>
-        <v>12000</v>
+        <f t="shared" si="5"/>
+        <v>12288</v>
       </c>
       <c r="I29" s="3">
-        <f t="shared" si="4"/>
-        <v>12000</v>
+        <f t="shared" si="6"/>
+        <v>12288</v>
       </c>
       <c r="J29" s="3">
-        <f>MOD(I29,$D$6)</f>
-        <v>12000</v>
+        <f t="shared" si="1"/>
+        <v>12288</v>
       </c>
       <c r="K29" s="2">
-        <f>J29/($D$6)</f>
-        <v>0.3662109375</v>
+        <f t="shared" si="2"/>
+        <v>0.375</v>
       </c>
       <c r="L29">
-        <f t="shared" si="5"/>
-        <v>12000</v>
+        <f t="shared" si="7"/>
+        <v>12288</v>
       </c>
       <c r="M29" s="2">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
     </row>
@@ -1448,39 +1469,39 @@
         <v>16</v>
       </c>
       <c r="B30" s="6">
-        <f t="shared" si="1"/>
-        <v>1.5625</v>
+        <f t="shared" si="3"/>
+        <v>1.6</v>
       </c>
       <c r="E30" s="2">
-        <f t="shared" si="2"/>
-        <v>0.390625</v>
+        <f t="shared" si="4"/>
+        <v>0.4</v>
       </c>
       <c r="F30" s="8">
         <f t="shared" si="0"/>
-        <v>0.63439328416364582</v>
+        <v>0.58778525229247325</v>
       </c>
       <c r="H30" s="2">
-        <f t="shared" si="3"/>
-        <v>12800</v>
+        <f t="shared" si="5"/>
+        <v>13107.2</v>
       </c>
       <c r="I30" s="3">
-        <f t="shared" si="4"/>
-        <v>12800</v>
+        <f t="shared" si="6"/>
+        <v>13107</v>
       </c>
       <c r="J30" s="3">
-        <f>MOD(I30,$D$6)</f>
-        <v>12800</v>
+        <f t="shared" si="1"/>
+        <v>13107</v>
       </c>
       <c r="K30" s="2">
-        <f>J30/($D$6)</f>
-        <v>0.390625</v>
+        <f t="shared" si="2"/>
+        <v>0.399993896484375</v>
       </c>
       <c r="L30">
-        <f t="shared" si="5"/>
-        <v>12800</v>
+        <f t="shared" si="7"/>
+        <v>13107</v>
       </c>
       <c r="M30" s="2">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
     </row>
@@ -1489,39 +1510,39 @@
         <v>17</v>
       </c>
       <c r="B31" s="6">
-        <f t="shared" si="1"/>
-        <v>1.66015625</v>
+        <f t="shared" si="3"/>
+        <v>1.7</v>
       </c>
       <c r="E31" s="2">
-        <f t="shared" si="2"/>
-        <v>0.4150390625</v>
+        <f t="shared" si="4"/>
+        <v>0.42499999999999999</v>
       </c>
       <c r="F31" s="8">
         <f t="shared" si="0"/>
-        <v>0.50883014254310732</v>
+        <v>0.45399049973954686</v>
       </c>
       <c r="H31" s="2">
-        <f t="shared" si="3"/>
-        <v>13600</v>
+        <f t="shared" si="5"/>
+        <v>13926.400000000001</v>
       </c>
       <c r="I31" s="3">
-        <f t="shared" si="4"/>
-        <v>13600</v>
+        <f t="shared" si="6"/>
+        <v>13926</v>
       </c>
       <c r="J31" s="3">
-        <f>MOD(I31,$D$6)</f>
-        <v>13600</v>
+        <f t="shared" si="1"/>
+        <v>13926</v>
       </c>
       <c r="K31" s="2">
-        <f>J31/($D$6)</f>
-        <v>0.4150390625</v>
+        <f t="shared" si="2"/>
+        <v>0.42498779296875</v>
       </c>
       <c r="L31">
-        <f t="shared" si="5"/>
-        <v>13600</v>
+        <f t="shared" si="7"/>
+        <v>13926</v>
       </c>
       <c r="M31" s="2">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
     </row>
@@ -1530,39 +1551,39 @@
         <v>18</v>
       </c>
       <c r="B32" s="6">
-        <f t="shared" si="1"/>
-        <v>1.7578125</v>
+        <f t="shared" si="3"/>
+        <v>1.8</v>
       </c>
       <c r="E32" s="2">
-        <f t="shared" si="2"/>
-        <v>0.439453125</v>
+        <f t="shared" si="4"/>
+        <v>0.45</v>
       </c>
       <c r="F32" s="8">
         <f t="shared" si="0"/>
-        <v>0.37131719395183771</v>
+        <v>0.30901699437494751</v>
       </c>
       <c r="H32" s="2">
-        <f t="shared" si="3"/>
-        <v>14400</v>
+        <f t="shared" si="5"/>
+        <v>14745.6</v>
       </c>
       <c r="I32" s="3">
-        <f t="shared" si="4"/>
-        <v>14400</v>
+        <f t="shared" si="6"/>
+        <v>14746</v>
       </c>
       <c r="J32" s="3">
-        <f>MOD(I32,$D$6)</f>
-        <v>14400</v>
+        <f t="shared" si="1"/>
+        <v>14746</v>
       </c>
       <c r="K32" s="2">
-        <f>J32/($D$6)</f>
-        <v>0.439453125</v>
+        <f t="shared" si="2"/>
+        <v>0.45001220703125</v>
       </c>
       <c r="L32">
-        <f t="shared" si="5"/>
-        <v>14400</v>
+        <f t="shared" si="7"/>
+        <v>14746</v>
       </c>
       <c r="M32" s="2">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
     </row>
@@ -1571,39 +1592,39 @@
         <v>19</v>
       </c>
       <c r="B33" s="6">
-        <f t="shared" si="1"/>
-        <v>1.85546875</v>
+        <f t="shared" si="3"/>
+        <v>1.9</v>
       </c>
       <c r="E33" s="2">
-        <f t="shared" si="2"/>
-        <v>0.4638671875</v>
+        <f t="shared" si="4"/>
+        <v>0.47499999999999998</v>
       </c>
       <c r="F33" s="8">
         <f t="shared" si="0"/>
-        <v>0.22508391135979328</v>
+        <v>0.15643446504023142</v>
       </c>
       <c r="H33" s="2">
-        <f t="shared" si="3"/>
-        <v>15200</v>
+        <f t="shared" si="5"/>
+        <v>15564.800000000001</v>
       </c>
       <c r="I33" s="3">
-        <f t="shared" si="4"/>
-        <v>15200</v>
+        <f t="shared" si="6"/>
+        <v>15565</v>
       </c>
       <c r="J33" s="3">
-        <f>MOD(I33,$D$6)</f>
-        <v>15200</v>
+        <f t="shared" si="1"/>
+        <v>15565</v>
       </c>
       <c r="K33" s="2">
-        <f>J33/($D$6)</f>
-        <v>0.4638671875</v>
+        <f t="shared" si="2"/>
+        <v>0.475006103515625</v>
       </c>
       <c r="L33">
-        <f t="shared" si="5"/>
-        <v>15200</v>
+        <f t="shared" si="7"/>
+        <v>15565</v>
       </c>
       <c r="M33" s="2">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
     </row>
@@ -1612,39 +1633,39 @@
         <v>20</v>
       </c>
       <c r="B34" s="6">
-        <f t="shared" si="1"/>
-        <v>1.953125</v>
+        <f t="shared" si="3"/>
+        <v>2</v>
       </c>
       <c r="E34" s="2">
-        <f t="shared" si="2"/>
-        <v>0.48828125</v>
+        <f t="shared" si="4"/>
+        <v>0.5</v>
       </c>
       <c r="F34" s="8">
         <f t="shared" si="0"/>
-        <v>7.3564563599667732E-2</v>
+        <v>1.22514845490862E-16</v>
       </c>
       <c r="H34" s="2">
-        <f t="shared" si="3"/>
-        <v>16000</v>
+        <f t="shared" si="5"/>
+        <v>16384</v>
       </c>
       <c r="I34" s="10">
-        <f t="shared" si="4"/>
-        <v>16000</v>
+        <f t="shared" si="6"/>
+        <v>16384</v>
       </c>
       <c r="J34" s="10">
-        <f>MOD(I34,$D$6)</f>
-        <v>16000</v>
+        <f t="shared" si="1"/>
+        <v>16384</v>
       </c>
       <c r="K34" s="9">
-        <f>J34/($D$6)</f>
-        <v>0.48828125</v>
+        <f t="shared" si="2"/>
+        <v>0.5</v>
       </c>
       <c r="L34" s="12">
-        <f t="shared" si="5"/>
-        <v>16000</v>
+        <f t="shared" si="7"/>
+        <v>16384</v>
       </c>
       <c r="M34" s="2">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
     </row>
@@ -1653,39 +1674,39 @@
         <v>21</v>
       </c>
       <c r="B35" s="6">
-        <f t="shared" si="1"/>
-        <v>2.05078125</v>
+        <f t="shared" si="3"/>
+        <v>2.1</v>
       </c>
       <c r="E35" s="2">
-        <f t="shared" si="2"/>
-        <v>0.5126953125</v>
+        <f t="shared" si="4"/>
+        <v>0.52500000000000002</v>
       </c>
       <c r="F35" s="8">
         <f t="shared" si="0"/>
-        <v>-7.9682437971429501E-2</v>
+        <v>-0.15643446504023073</v>
       </c>
       <c r="H35" s="2">
-        <f t="shared" si="3"/>
-        <v>16800</v>
+        <f t="shared" si="5"/>
+        <v>17203.2</v>
       </c>
       <c r="I35" s="3">
-        <f t="shared" si="4"/>
-        <v>16800</v>
+        <f t="shared" si="6"/>
+        <v>17203</v>
       </c>
       <c r="J35" s="3">
-        <f>MOD(I35,$D$6)</f>
-        <v>16800</v>
+        <f t="shared" si="1"/>
+        <v>17203</v>
       </c>
       <c r="K35" s="2">
-        <f>J35/($D$6)</f>
-        <v>0.5126953125</v>
+        <f t="shared" si="2"/>
+        <v>0.524993896484375</v>
       </c>
       <c r="L35">
-        <f t="shared" si="5"/>
-        <v>16800</v>
+        <f t="shared" si="7"/>
+        <v>17203</v>
       </c>
       <c r="M35" s="2">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
     </row>
@@ -1694,39 +1715,39 @@
         <v>22</v>
       </c>
       <c r="B36" s="6">
-        <f t="shared" si="1"/>
-        <v>2.1484375</v>
+        <f t="shared" si="3"/>
+        <v>2.2000000000000002</v>
       </c>
       <c r="E36" s="2">
-        <f t="shared" si="2"/>
-        <v>0.537109375</v>
+        <f t="shared" si="4"/>
+        <v>0.55000000000000004</v>
       </c>
       <c r="F36" s="8">
         <f t="shared" si="0"/>
-        <v>-0.23105810828067108</v>
+        <v>-0.30901699437494728</v>
       </c>
       <c r="H36" s="2">
-        <f t="shared" si="3"/>
-        <v>17600</v>
+        <f t="shared" si="5"/>
+        <v>18022.400000000001</v>
       </c>
       <c r="I36" s="3">
-        <f t="shared" si="4"/>
-        <v>17600</v>
+        <f t="shared" si="6"/>
+        <v>18022</v>
       </c>
       <c r="J36" s="3">
-        <f>MOD(I36,$D$6)</f>
-        <v>17600</v>
+        <f t="shared" si="1"/>
+        <v>18022</v>
       </c>
       <c r="K36" s="2">
-        <f>J36/($D$6)</f>
-        <v>0.537109375</v>
+        <f t="shared" si="2"/>
+        <v>0.54998779296875</v>
       </c>
       <c r="L36">
-        <f t="shared" si="5"/>
-        <v>17600</v>
+        <f t="shared" si="7"/>
+        <v>18022</v>
       </c>
       <c r="M36" s="2">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
     </row>
@@ -1735,39 +1756,39 @@
         <v>23</v>
       </c>
       <c r="B37" s="6">
-        <f t="shared" si="1"/>
-        <v>2.24609375</v>
+        <f t="shared" si="3"/>
+        <v>2.2999999999999998</v>
       </c>
       <c r="E37" s="2">
-        <f t="shared" si="2"/>
-        <v>0.5615234375</v>
+        <f t="shared" si="4"/>
+        <v>0.57499999999999996</v>
       </c>
       <c r="F37" s="8">
         <f t="shared" si="0"/>
-        <v>-0.37700741021641793</v>
+        <v>-0.45399049973954625</v>
       </c>
       <c r="H37" s="2">
-        <f t="shared" si="3"/>
-        <v>18400</v>
+        <f t="shared" si="5"/>
+        <v>18841.600000000002</v>
       </c>
       <c r="I37" s="3">
-        <f t="shared" si="4"/>
-        <v>18400</v>
+        <f t="shared" si="6"/>
+        <v>18842</v>
       </c>
       <c r="J37" s="3">
-        <f>MOD(I37,$D$6)</f>
-        <v>18400</v>
+        <f t="shared" si="1"/>
+        <v>18842</v>
       </c>
       <c r="K37" s="2">
-        <f>J37/($D$6)</f>
-        <v>0.5615234375</v>
+        <f t="shared" si="2"/>
+        <v>0.57501220703125</v>
       </c>
       <c r="L37">
-        <f t="shared" si="5"/>
-        <v>18400</v>
+        <f t="shared" si="7"/>
+        <v>18842</v>
       </c>
       <c r="M37" s="2">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
     </row>
@@ -1776,39 +1797,39 @@
         <v>24</v>
       </c>
       <c r="B38" s="6">
-        <f t="shared" si="1"/>
-        <v>2.34375</v>
+        <f t="shared" si="3"/>
+        <v>2.4</v>
       </c>
       <c r="E38" s="2">
-        <f t="shared" si="2"/>
-        <v>0.5859375</v>
+        <f t="shared" si="4"/>
+        <v>0.6</v>
       </c>
       <c r="F38" s="8">
         <f t="shared" si="0"/>
-        <v>-0.51410274419322155</v>
+        <v>-0.58778525229247269</v>
       </c>
       <c r="H38" s="2">
-        <f t="shared" si="3"/>
-        <v>19200</v>
+        <f t="shared" si="5"/>
+        <v>19660.800000000003</v>
       </c>
       <c r="I38" s="3">
-        <f t="shared" si="4"/>
-        <v>19200</v>
+        <f t="shared" si="6"/>
+        <v>19661</v>
       </c>
       <c r="J38" s="3">
-        <f>MOD(I38,$D$6)</f>
-        <v>19200</v>
+        <f t="shared" si="1"/>
+        <v>19661</v>
       </c>
       <c r="K38" s="2">
-        <f>J38/($D$6)</f>
-        <v>0.5859375</v>
+        <f t="shared" si="2"/>
+        <v>0.600006103515625</v>
       </c>
       <c r="L38">
-        <f t="shared" si="5"/>
-        <v>19200</v>
+        <f t="shared" si="7"/>
+        <v>19661</v>
       </c>
       <c r="M38" s="2">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
     </row>
@@ -1817,39 +1838,39 @@
         <v>25</v>
       </c>
       <c r="B39" s="6">
-        <f t="shared" si="1"/>
-        <v>2.44140625</v>
+        <f t="shared" si="3"/>
+        <v>2.5</v>
       </c>
       <c r="E39" s="2">
-        <f t="shared" si="2"/>
-        <v>0.6103515625</v>
+        <f t="shared" si="4"/>
+        <v>0.625</v>
       </c>
       <c r="F39" s="8">
         <f t="shared" si="0"/>
-        <v>-0.6391244448637754</v>
+        <v>-0.70710678118654713</v>
       </c>
       <c r="H39" s="2">
-        <f t="shared" si="3"/>
-        <v>20000</v>
+        <f t="shared" si="5"/>
+        <v>20480</v>
       </c>
       <c r="I39" s="3">
-        <f t="shared" si="4"/>
-        <v>20000</v>
+        <f t="shared" si="6"/>
+        <v>20480</v>
       </c>
       <c r="J39" s="3">
-        <f>MOD(I39,$D$6)</f>
-        <v>20000</v>
+        <f t="shared" si="1"/>
+        <v>20480</v>
       </c>
       <c r="K39" s="2">
-        <f>J39/($D$6)</f>
-        <v>0.6103515625</v>
+        <f t="shared" si="2"/>
+        <v>0.625</v>
       </c>
       <c r="L39">
-        <f t="shared" si="5"/>
-        <v>20000</v>
+        <f t="shared" si="7"/>
+        <v>20480</v>
       </c>
       <c r="M39" s="2">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
     </row>
@@ -1858,39 +1879,39 @@
         <v>26</v>
       </c>
       <c r="B40" s="6">
-        <f t="shared" ref="B40:B59" si="7">A40*1/$C$3*1000</f>
-        <v>2.5390625</v>
+        <f t="shared" ref="B40:B59" si="9">A40*1/$C$3*1000</f>
+        <v>2.6</v>
       </c>
       <c r="E40" s="2">
-        <f t="shared" ref="E40:E59" si="8">$C$5*B40/1000</f>
-        <v>0.634765625</v>
+        <f t="shared" ref="E40:E59" si="10">$C$5*B40/1000</f>
+        <v>0.65</v>
       </c>
       <c r="F40" s="8">
-        <f t="shared" ref="F40:F59" si="9">SIN(2*PI()*$C$5*B40/1000)</f>
-        <v>-0.74913639452345882</v>
+        <f t="shared" ref="F40:F59" si="11">SIN(2*PI()*$C$5*B40/1000)</f>
+        <v>-0.80901699437494734</v>
       </c>
       <c r="H40" s="2">
-        <f t="shared" ref="H40:H59" si="10">$J$4*A40</f>
-        <v>20800</v>
+        <f t="shared" ref="H40:H59" si="12">$J$4*A40</f>
+        <v>21299.200000000001</v>
       </c>
       <c r="I40" s="3">
-        <f t="shared" si="4"/>
-        <v>20800</v>
+        <f t="shared" si="6"/>
+        <v>21299</v>
       </c>
       <c r="J40" s="3">
-        <f t="shared" ref="J40:J54" si="11">MOD(I40,$D$6)</f>
-        <v>20800</v>
+        <f t="shared" ref="J40:J54" si="13">MOD(I40,$D$6)</f>
+        <v>21299</v>
       </c>
       <c r="K40" s="2">
-        <f t="shared" ref="K40:K54" si="12">J40/($D$6)</f>
-        <v>0.634765625</v>
+        <f t="shared" ref="K40:K54" si="14">J40/($D$6)</f>
+        <v>0.649993896484375</v>
       </c>
       <c r="L40">
-        <f t="shared" ref="L40:L59" si="13">_xlfn.BITAND(I40,$D$6-1)</f>
-        <v>20800</v>
+        <f t="shared" ref="L40:L59" si="15">_xlfn.BITAND(I40,$D$6-1)</f>
+        <v>21299</v>
       </c>
       <c r="M40" s="2">
-        <f t="shared" ref="M40:M59" si="14">$L$4*B40/1000</f>
+        <f t="shared" ref="M40:M59" si="16">$L$4*B40/1000</f>
         <v>0</v>
       </c>
     </row>
@@ -1899,39 +1920,39 @@
         <v>27</v>
       </c>
       <c r="B41" s="6">
-        <f t="shared" si="7"/>
-        <v>2.63671875</v>
+        <f t="shared" si="9"/>
+        <v>2.7</v>
       </c>
       <c r="E41" s="2">
-        <f t="shared" si="8"/>
-        <v>0.6591796875</v>
+        <f t="shared" si="10"/>
+        <v>0.67500000000000004</v>
       </c>
       <c r="F41" s="8">
-        <f t="shared" si="9"/>
-        <v>-0.841554977436898</v>
+        <f t="shared" si="11"/>
+        <v>-0.89100652418836779</v>
       </c>
       <c r="H41" s="2">
-        <f t="shared" si="10"/>
-        <v>21600</v>
+        <f t="shared" si="12"/>
+        <v>22118.400000000001</v>
       </c>
       <c r="I41" s="3">
-        <f t="shared" si="4"/>
-        <v>21600</v>
+        <f t="shared" si="6"/>
+        <v>22118</v>
       </c>
       <c r="J41" s="3">
-        <f t="shared" si="11"/>
-        <v>21600</v>
+        <f t="shared" si="13"/>
+        <v>22118</v>
       </c>
       <c r="K41" s="2">
-        <f t="shared" si="12"/>
-        <v>0.6591796875</v>
+        <f t="shared" si="14"/>
+        <v>0.67498779296875</v>
       </c>
       <c r="L41">
-        <f t="shared" si="13"/>
-        <v>21600</v>
+        <f t="shared" si="15"/>
+        <v>22118</v>
       </c>
       <c r="M41" s="2">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
     </row>
@@ -1940,39 +1961,39 @@
         <v>28</v>
       </c>
       <c r="B42" s="6">
-        <f t="shared" si="7"/>
-        <v>2.734375</v>
+        <f t="shared" si="9"/>
+        <v>2.8</v>
       </c>
       <c r="E42" s="2">
-        <f t="shared" si="8"/>
-        <v>0.68359375</v>
+        <f t="shared" si="10"/>
+        <v>0.7</v>
       </c>
       <c r="F42" s="8">
-        <f t="shared" si="9"/>
-        <v>-0.91420975570353047</v>
+        <f t="shared" si="11"/>
+        <v>-0.95105651629515353</v>
       </c>
       <c r="H42" s="2">
-        <f t="shared" si="10"/>
-        <v>22400</v>
+        <f t="shared" si="12"/>
+        <v>22937.600000000002</v>
       </c>
       <c r="I42" s="3">
-        <f t="shared" si="4"/>
-        <v>22400</v>
+        <f t="shared" si="6"/>
+        <v>22938</v>
       </c>
       <c r="J42" s="3">
-        <f t="shared" si="11"/>
-        <v>22400</v>
+        <f t="shared" si="13"/>
+        <v>22938</v>
       </c>
       <c r="K42" s="2">
-        <f t="shared" si="12"/>
-        <v>0.68359375</v>
+        <f t="shared" si="14"/>
+        <v>0.70001220703125</v>
       </c>
       <c r="L42">
-        <f t="shared" si="13"/>
-        <v>22400</v>
+        <f t="shared" si="15"/>
+        <v>22938</v>
       </c>
       <c r="M42" s="2">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
     </row>
@@ -1981,39 +2002,39 @@
         <v>29</v>
       </c>
       <c r="B43" s="6">
-        <f t="shared" si="7"/>
-        <v>2.83203125</v>
+        <f t="shared" si="9"/>
+        <v>2.9</v>
       </c>
       <c r="E43" s="2">
-        <f t="shared" si="8"/>
-        <v>0.7080078125</v>
+        <f t="shared" si="10"/>
+        <v>0.72499999999999998</v>
       </c>
       <c r="F43" s="8">
-        <f t="shared" si="9"/>
-        <v>-0.96539444169768929</v>
+        <f t="shared" si="11"/>
+        <v>-0.98768834059513766</v>
       </c>
       <c r="H43" s="2">
-        <f t="shared" si="10"/>
-        <v>23200</v>
+        <f t="shared" si="12"/>
+        <v>23756.800000000003</v>
       </c>
       <c r="I43" s="3">
-        <f t="shared" si="4"/>
-        <v>23200</v>
+        <f t="shared" si="6"/>
+        <v>23757</v>
       </c>
       <c r="J43" s="3">
-        <f t="shared" si="11"/>
-        <v>23200</v>
+        <f t="shared" si="13"/>
+        <v>23757</v>
       </c>
       <c r="K43" s="2">
-        <f t="shared" si="12"/>
-        <v>0.7080078125</v>
+        <f t="shared" si="14"/>
+        <v>0.725006103515625</v>
       </c>
       <c r="L43">
-        <f t="shared" si="13"/>
-        <v>23200</v>
+        <f t="shared" si="15"/>
+        <v>23757</v>
       </c>
       <c r="M43" s="2">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
     </row>
@@ -2022,39 +2043,39 @@
         <v>30</v>
       </c>
       <c r="B44" s="6">
-        <f t="shared" si="7"/>
-        <v>2.9296875</v>
+        <f t="shared" si="9"/>
+        <v>3</v>
       </c>
       <c r="E44" s="2">
-        <f t="shared" si="8"/>
-        <v>0.732421875</v>
+        <f t="shared" si="10"/>
+        <v>0.75</v>
       </c>
       <c r="F44" s="8">
-        <f t="shared" si="9"/>
-        <v>-0.99390697000235606</v>
+        <f t="shared" si="11"/>
+        <v>-1</v>
       </c>
       <c r="H44" s="2">
-        <f t="shared" si="10"/>
-        <v>24000</v>
+        <f t="shared" si="12"/>
+        <v>24576</v>
       </c>
       <c r="I44" s="3">
-        <f t="shared" si="4"/>
-        <v>24000</v>
+        <f t="shared" si="6"/>
+        <v>24576</v>
       </c>
       <c r="J44" s="3">
-        <f t="shared" si="11"/>
-        <v>24000</v>
+        <f t="shared" si="13"/>
+        <v>24576</v>
       </c>
       <c r="K44" s="2">
-        <f t="shared" si="12"/>
-        <v>0.732421875</v>
+        <f t="shared" si="14"/>
+        <v>0.75</v>
       </c>
       <c r="L44">
-        <f t="shared" si="13"/>
-        <v>24000</v>
+        <f t="shared" si="15"/>
+        <v>24576</v>
       </c>
       <c r="M44" s="2">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
     </row>
@@ -2063,39 +2084,39 @@
         <v>31</v>
       </c>
       <c r="B45" s="6">
-        <f t="shared" si="7"/>
-        <v>3.02734375</v>
+        <f t="shared" si="9"/>
+        <v>3.1</v>
       </c>
       <c r="E45" s="2">
-        <f t="shared" si="8"/>
-        <v>0.7568359375</v>
+        <f t="shared" si="10"/>
+        <v>0.77500000000000002</v>
       </c>
       <c r="F45" s="8">
-        <f t="shared" si="9"/>
-        <v>-0.99907772775264536</v>
+        <f t="shared" si="11"/>
+        <v>-0.98768834059513777</v>
       </c>
       <c r="H45" s="2">
-        <f t="shared" si="10"/>
-        <v>24800</v>
+        <f t="shared" si="12"/>
+        <v>25395.200000000001</v>
       </c>
       <c r="I45" s="3">
-        <f t="shared" si="4"/>
-        <v>24800</v>
+        <f t="shared" si="6"/>
+        <v>25395</v>
       </c>
       <c r="J45" s="3">
-        <f t="shared" si="11"/>
-        <v>24800</v>
+        <f t="shared" si="13"/>
+        <v>25395</v>
       </c>
       <c r="K45" s="2">
-        <f t="shared" si="12"/>
-        <v>0.7568359375</v>
+        <f t="shared" si="14"/>
+        <v>0.774993896484375</v>
       </c>
       <c r="L45">
-        <f t="shared" si="13"/>
-        <v>24800</v>
+        <f t="shared" si="15"/>
+        <v>25395</v>
       </c>
       <c r="M45" s="2">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
     </row>
@@ -2104,39 +2125,39 @@
         <v>32</v>
       </c>
       <c r="B46" s="6">
-        <f t="shared" si="7"/>
-        <v>3.125</v>
+        <f t="shared" si="9"/>
+        <v>3.2</v>
       </c>
       <c r="E46" s="2">
-        <f t="shared" si="8"/>
-        <v>0.78125</v>
+        <f t="shared" si="10"/>
+        <v>0.8</v>
       </c>
       <c r="F46" s="8">
-        <f t="shared" si="9"/>
-        <v>-0.98078528040323065</v>
+        <f t="shared" si="11"/>
+        <v>-0.95105651629515364</v>
       </c>
       <c r="H46" s="2">
-        <f t="shared" si="10"/>
-        <v>25600</v>
+        <f t="shared" si="12"/>
+        <v>26214.400000000001</v>
       </c>
       <c r="I46" s="3">
-        <f t="shared" si="4"/>
-        <v>25600</v>
+        <f t="shared" si="6"/>
+        <v>26214</v>
       </c>
       <c r="J46" s="3">
-        <f t="shared" si="11"/>
-        <v>25600</v>
+        <f t="shared" si="13"/>
+        <v>26214</v>
       </c>
       <c r="K46" s="2">
-        <f t="shared" si="12"/>
-        <v>0.78125</v>
+        <f t="shared" si="14"/>
+        <v>0.79998779296875</v>
       </c>
       <c r="L46">
-        <f t="shared" si="13"/>
-        <v>25600</v>
+        <f t="shared" si="15"/>
+        <v>26214</v>
       </c>
       <c r="M46" s="2">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
     </row>
@@ -2145,39 +2166,39 @@
         <v>33</v>
       </c>
       <c r="B47" s="6">
-        <f t="shared" si="7"/>
-        <v>3.22265625</v>
+        <f t="shared" si="9"/>
+        <v>3.3</v>
       </c>
       <c r="E47" s="2">
-        <f t="shared" si="8"/>
-        <v>0.8056640625</v>
+        <f t="shared" si="10"/>
+        <v>0.82499999999999996</v>
       </c>
       <c r="F47" s="8">
-        <f t="shared" si="9"/>
-        <v>-0.93945922360219014</v>
+        <f t="shared" si="11"/>
+        <v>-0.89100652418836834</v>
       </c>
       <c r="H47" s="2">
-        <f t="shared" si="10"/>
-        <v>26400</v>
+        <f t="shared" si="12"/>
+        <v>27033.600000000002</v>
       </c>
       <c r="I47" s="3">
-        <f t="shared" si="4"/>
-        <v>26400</v>
+        <f t="shared" si="6"/>
+        <v>27034</v>
       </c>
       <c r="J47" s="3">
-        <f t="shared" si="11"/>
-        <v>26400</v>
+        <f t="shared" si="13"/>
+        <v>27034</v>
       </c>
       <c r="K47" s="2">
-        <f t="shared" si="12"/>
-        <v>0.8056640625</v>
+        <f t="shared" si="14"/>
+        <v>0.82501220703125</v>
       </c>
       <c r="L47">
-        <f t="shared" si="13"/>
-        <v>26400</v>
+        <f t="shared" si="15"/>
+        <v>27034</v>
       </c>
       <c r="M47" s="2">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
     </row>
@@ -2186,39 +2207,39 @@
         <v>34</v>
       </c>
       <c r="B48" s="6">
-        <f t="shared" si="7"/>
-        <v>3.3203125</v>
+        <f t="shared" si="9"/>
+        <v>3.4</v>
       </c>
       <c r="E48" s="2">
-        <f t="shared" si="8"/>
-        <v>0.830078125</v>
+        <f t="shared" si="10"/>
+        <v>0.85</v>
       </c>
       <c r="F48" s="8">
-        <f t="shared" si="9"/>
-        <v>-0.87607009419540693</v>
+        <f t="shared" si="11"/>
+        <v>-0.80901699437494756</v>
       </c>
       <c r="H48" s="2">
-        <f t="shared" si="10"/>
-        <v>27200</v>
+        <f t="shared" si="12"/>
+        <v>27852.800000000003</v>
       </c>
       <c r="I48" s="3">
-        <f t="shared" si="4"/>
-        <v>27200</v>
+        <f t="shared" si="6"/>
+        <v>27853</v>
       </c>
       <c r="J48" s="3">
-        <f t="shared" si="11"/>
-        <v>27200</v>
+        <f t="shared" si="13"/>
+        <v>27853</v>
       </c>
       <c r="K48" s="2">
-        <f t="shared" si="12"/>
-        <v>0.830078125</v>
+        <f t="shared" si="14"/>
+        <v>0.850006103515625</v>
       </c>
       <c r="L48">
-        <f t="shared" si="13"/>
-        <v>27200</v>
+        <f t="shared" si="15"/>
+        <v>27853</v>
       </c>
       <c r="M48" s="2">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
     </row>
@@ -2227,39 +2248,39 @@
         <v>35</v>
       </c>
       <c r="B49" s="6">
-        <f t="shared" si="7"/>
-        <v>3.41796875</v>
+        <f t="shared" si="9"/>
+        <v>3.5</v>
       </c>
       <c r="E49" s="2">
-        <f t="shared" si="8"/>
-        <v>0.8544921875</v>
+        <f t="shared" si="10"/>
+        <v>0.875</v>
       </c>
       <c r="F49" s="8">
-        <f t="shared" si="9"/>
-        <v>-0.79210657730021261</v>
+        <f t="shared" si="11"/>
+        <v>-0.70710678118654768</v>
       </c>
       <c r="H49" s="2">
-        <f t="shared" si="10"/>
-        <v>28000</v>
+        <f t="shared" si="12"/>
+        <v>28672</v>
       </c>
       <c r="I49" s="3">
-        <f t="shared" si="4"/>
-        <v>28000</v>
+        <f t="shared" si="6"/>
+        <v>28672</v>
       </c>
       <c r="J49" s="3">
-        <f t="shared" si="11"/>
-        <v>28000</v>
+        <f t="shared" si="13"/>
+        <v>28672</v>
       </c>
       <c r="K49" s="2">
-        <f t="shared" si="12"/>
-        <v>0.8544921875</v>
+        <f t="shared" si="14"/>
+        <v>0.875</v>
       </c>
       <c r="L49">
-        <f t="shared" si="13"/>
-        <v>28000</v>
+        <f t="shared" si="15"/>
+        <v>28672</v>
       </c>
       <c r="M49" s="2">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
     </row>
@@ -2268,39 +2289,39 @@
         <v>36</v>
       </c>
       <c r="B50" s="6">
-        <f t="shared" si="7"/>
-        <v>3.515625</v>
+        <f t="shared" si="9"/>
+        <v>3.6</v>
       </c>
       <c r="E50" s="2">
-        <f t="shared" si="8"/>
-        <v>0.87890625</v>
+        <f t="shared" si="10"/>
+        <v>0.9</v>
       </c>
       <c r="F50" s="8">
-        <f t="shared" si="9"/>
-        <v>-0.68954054473706716</v>
+        <f t="shared" si="11"/>
+        <v>-0.58778525229247336</v>
       </c>
       <c r="H50" s="2">
-        <f t="shared" si="10"/>
-        <v>28800</v>
+        <f t="shared" si="12"/>
+        <v>29491.200000000001</v>
       </c>
       <c r="I50" s="3">
-        <f t="shared" si="4"/>
-        <v>28800</v>
+        <f t="shared" si="6"/>
+        <v>29491</v>
       </c>
       <c r="J50" s="3">
-        <f t="shared" si="11"/>
-        <v>28800</v>
+        <f t="shared" si="13"/>
+        <v>29491</v>
       </c>
       <c r="K50" s="2">
-        <f t="shared" si="12"/>
-        <v>0.87890625</v>
+        <f t="shared" si="14"/>
+        <v>0.899993896484375</v>
       </c>
       <c r="L50">
-        <f t="shared" si="13"/>
-        <v>28800</v>
+        <f t="shared" si="15"/>
+        <v>29491</v>
       </c>
       <c r="M50" s="2">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
     </row>
@@ -2309,39 +2330,39 @@
         <v>37</v>
       </c>
       <c r="B51" s="6">
-        <f t="shared" si="7"/>
-        <v>3.61328125</v>
+        <f t="shared" si="9"/>
+        <v>3.7</v>
       </c>
       <c r="E51" s="2">
-        <f t="shared" si="8"/>
-        <v>0.9033203125</v>
+        <f t="shared" si="10"/>
+        <v>0.92500000000000004</v>
       </c>
       <c r="F51" s="8">
-        <f t="shared" si="9"/>
-        <v>-0.57078074588696814</v>
+        <f t="shared" si="11"/>
+        <v>-0.45399049973954697</v>
       </c>
       <c r="H51" s="2">
-        <f t="shared" si="10"/>
-        <v>29600</v>
+        <f t="shared" si="12"/>
+        <v>30310.400000000001</v>
       </c>
       <c r="I51" s="3">
-        <f t="shared" si="4"/>
-        <v>29600</v>
+        <f t="shared" si="6"/>
+        <v>30310</v>
       </c>
       <c r="J51" s="3">
-        <f t="shared" si="11"/>
-        <v>29600</v>
+        <f t="shared" si="13"/>
+        <v>30310</v>
       </c>
       <c r="K51" s="2">
-        <f t="shared" si="12"/>
-        <v>0.9033203125</v>
+        <f t="shared" si="14"/>
+        <v>0.92498779296875</v>
       </c>
       <c r="L51">
-        <f t="shared" si="13"/>
-        <v>29600</v>
+        <f t="shared" si="15"/>
+        <v>30310</v>
       </c>
       <c r="M51" s="2">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
     </row>
@@ -2350,39 +2371,39 @@
         <v>38</v>
       </c>
       <c r="B52" s="6">
-        <f t="shared" si="7"/>
-        <v>3.7109375</v>
+        <f t="shared" si="9"/>
+        <v>3.8</v>
       </c>
       <c r="E52" s="2">
-        <f t="shared" si="8"/>
-        <v>0.927734375</v>
+        <f t="shared" si="10"/>
+        <v>0.95</v>
       </c>
       <c r="F52" s="8">
-        <f t="shared" si="9"/>
-        <v>-0.43861623853852844</v>
+        <f t="shared" si="11"/>
+        <v>-0.30901699437494851</v>
       </c>
       <c r="H52" s="2">
-        <f t="shared" si="10"/>
-        <v>30400</v>
+        <f t="shared" si="12"/>
+        <v>31129.600000000002</v>
       </c>
       <c r="I52" s="3">
-        <f t="shared" si="4"/>
-        <v>30400</v>
+        <f t="shared" si="6"/>
+        <v>31130</v>
       </c>
       <c r="J52" s="3">
-        <f t="shared" si="11"/>
-        <v>30400</v>
+        <f t="shared" si="13"/>
+        <v>31130</v>
       </c>
       <c r="K52" s="2">
-        <f t="shared" si="12"/>
-        <v>0.927734375</v>
+        <f t="shared" si="14"/>
+        <v>0.95001220703125</v>
       </c>
       <c r="L52">
-        <f t="shared" si="13"/>
-        <v>30400</v>
+        <f t="shared" si="15"/>
+        <v>31130</v>
       </c>
       <c r="M52" s="2">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
     </row>
@@ -2391,39 +2412,39 @@
         <v>39</v>
       </c>
       <c r="B53" s="6">
-        <f t="shared" si="7"/>
-        <v>3.80859375</v>
+        <f t="shared" si="9"/>
+        <v>3.9</v>
       </c>
       <c r="E53" s="2">
-        <f t="shared" si="8"/>
-        <v>0.9521484375</v>
+        <f t="shared" si="10"/>
+        <v>0.97499999999999998</v>
       </c>
       <c r="F53" s="8">
-        <f t="shared" si="9"/>
-        <v>-0.29615088824362373</v>
+        <f t="shared" si="11"/>
+        <v>-0.15643446504023198</v>
       </c>
       <c r="H53" s="2">
-        <f t="shared" si="10"/>
-        <v>31200</v>
+        <f t="shared" si="12"/>
+        <v>31948.800000000003</v>
       </c>
       <c r="I53" s="3">
-        <f t="shared" si="4"/>
-        <v>31200</v>
+        <f t="shared" si="6"/>
+        <v>31949</v>
       </c>
       <c r="J53" s="3">
-        <f t="shared" si="11"/>
-        <v>31200</v>
+        <f t="shared" si="13"/>
+        <v>31949</v>
       </c>
       <c r="K53" s="2">
-        <f t="shared" si="12"/>
-        <v>0.9521484375</v>
+        <f t="shared" si="14"/>
+        <v>0.975006103515625</v>
       </c>
       <c r="L53">
-        <f t="shared" si="13"/>
-        <v>31200</v>
+        <f t="shared" si="15"/>
+        <v>31949</v>
       </c>
       <c r="M53" s="2">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
     </row>
@@ -2432,39 +2453,39 @@
         <v>40</v>
       </c>
       <c r="B54" s="6">
-        <f t="shared" si="7"/>
-        <v>3.90625</v>
+        <f t="shared" si="9"/>
+        <v>4</v>
       </c>
       <c r="E54" s="2">
-        <f t="shared" si="8"/>
-        <v>0.9765625</v>
+        <f t="shared" si="10"/>
+        <v>1</v>
       </c>
       <c r="F54" s="8">
-        <f t="shared" si="9"/>
-        <v>-0.14673047445536239</v>
+        <f t="shared" si="11"/>
+        <v>-2.45029690981724E-16</v>
       </c>
       <c r="H54" s="2">
-        <f t="shared" si="10"/>
-        <v>32000</v>
+        <f t="shared" si="12"/>
+        <v>32768</v>
       </c>
       <c r="I54" s="3">
-        <f t="shared" si="4"/>
-        <v>32000</v>
+        <f t="shared" si="6"/>
+        <v>32768</v>
       </c>
       <c r="J54" s="3">
-        <f t="shared" si="11"/>
-        <v>32000</v>
+        <f t="shared" si="13"/>
+        <v>0</v>
       </c>
       <c r="K54" s="2">
-        <f t="shared" si="12"/>
-        <v>0.9765625</v>
+        <f t="shared" si="14"/>
+        <v>0</v>
       </c>
       <c r="L54">
-        <f t="shared" si="13"/>
-        <v>32000</v>
+        <f t="shared" si="15"/>
+        <v>0</v>
       </c>
       <c r="M54" s="2">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
     </row>
@@ -2473,39 +2494,39 @@
         <v>41</v>
       </c>
       <c r="B55" s="6">
-        <f t="shared" si="7"/>
-        <v>4.00390625</v>
+        <f t="shared" si="9"/>
+        <v>4.1000000000000005</v>
       </c>
       <c r="E55" s="2">
-        <f t="shared" si="8"/>
-        <v>1.0009765625</v>
+        <f t="shared" si="10"/>
+        <v>1.0250000000000001</v>
       </c>
       <c r="F55" s="8">
-        <f t="shared" si="9"/>
-        <v>6.1358846491539869E-3</v>
+        <f t="shared" si="11"/>
+        <v>0.15643446504023151</v>
       </c>
       <c r="H55" s="2">
-        <f t="shared" si="10"/>
-        <v>32800</v>
+        <f t="shared" si="12"/>
+        <v>33587.200000000004</v>
       </c>
       <c r="I55" s="3">
-        <f t="shared" si="4"/>
-        <v>32800</v>
+        <f t="shared" si="6"/>
+        <v>33587</v>
       </c>
       <c r="J55" s="3">
         <f>MOD(I55,$D$6)</f>
-        <v>32</v>
+        <v>819</v>
       </c>
       <c r="K55" s="2">
         <f>J55/($D$6)</f>
-        <v>9.765625E-4</v>
+        <v>2.4993896484375E-2</v>
       </c>
       <c r="L55">
-        <f t="shared" si="13"/>
-        <v>32</v>
+        <f t="shared" si="15"/>
+        <v>819</v>
       </c>
       <c r="M55" s="2">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
     </row>
@@ -2514,39 +2535,39 @@
         <v>42</v>
       </c>
       <c r="B56" s="6">
-        <f t="shared" si="7"/>
-        <v>4.1015625</v>
+        <f t="shared" si="9"/>
+        <v>4.2</v>
       </c>
       <c r="E56" s="2">
-        <f t="shared" si="8"/>
-        <v>1.025390625</v>
+        <f t="shared" si="10"/>
+        <v>1.05</v>
       </c>
       <c r="F56" s="8">
-        <f t="shared" si="9"/>
-        <v>0.15885814333386022</v>
+        <f t="shared" si="11"/>
+        <v>0.30901699437494717</v>
       </c>
       <c r="H56" s="2">
-        <f t="shared" si="10"/>
-        <v>33600</v>
+        <f t="shared" si="12"/>
+        <v>34406.400000000001</v>
       </c>
       <c r="I56" s="3">
-        <f t="shared" si="4"/>
-        <v>33600</v>
+        <f t="shared" si="6"/>
+        <v>34406</v>
       </c>
       <c r="J56" s="3">
         <f>MOD(I56,$D$6)</f>
-        <v>832</v>
+        <v>1638</v>
       </c>
       <c r="K56" s="2">
         <f>J56/($D$6)</f>
-        <v>2.5390625E-2</v>
+        <v>4.998779296875E-2</v>
       </c>
       <c r="L56">
-        <f t="shared" si="13"/>
-        <v>832</v>
+        <f t="shared" si="15"/>
+        <v>1638</v>
       </c>
       <c r="M56" s="2">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
     </row>
@@ -2555,39 +2576,39 @@
         <v>43</v>
       </c>
       <c r="B57" s="6">
-        <f t="shared" si="7"/>
-        <v>4.19921875</v>
+        <f t="shared" si="9"/>
+        <v>4.3</v>
       </c>
       <c r="E57" s="2">
-        <f t="shared" si="8"/>
-        <v>1.0498046875</v>
+        <f t="shared" si="10"/>
+        <v>1.075</v>
       </c>
       <c r="F57" s="8">
-        <f t="shared" si="9"/>
-        <v>0.30784964004153387</v>
+        <f t="shared" si="11"/>
+        <v>0.45399049973954575</v>
       </c>
       <c r="H57" s="2">
-        <f t="shared" si="10"/>
-        <v>34400</v>
+        <f t="shared" si="12"/>
+        <v>35225.599999999999</v>
       </c>
       <c r="I57" s="3">
-        <f t="shared" si="4"/>
-        <v>34400</v>
+        <f t="shared" si="6"/>
+        <v>35226</v>
       </c>
       <c r="J57" s="3">
         <f>MOD(I57,$D$6)</f>
-        <v>1632</v>
+        <v>2458</v>
       </c>
       <c r="K57" s="2">
         <f>J57/($D$6)</f>
-        <v>4.98046875E-2</v>
+        <v>7.501220703125E-2</v>
       </c>
       <c r="L57">
-        <f t="shared" si="13"/>
-        <v>1632</v>
+        <f t="shared" si="15"/>
+        <v>2458</v>
       </c>
       <c r="M57" s="2">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
     </row>
@@ -2596,39 +2617,39 @@
         <v>44</v>
       </c>
       <c r="B58" s="6">
-        <f t="shared" si="7"/>
-        <v>4.296875</v>
+        <f t="shared" si="9"/>
+        <v>4.4000000000000004</v>
       </c>
       <c r="E58" s="2">
-        <f t="shared" si="8"/>
-        <v>1.07421875</v>
+        <f t="shared" si="10"/>
+        <v>1.1000000000000001</v>
       </c>
       <c r="F58" s="8">
-        <f t="shared" si="9"/>
-        <v>0.44961132965460654</v>
+        <f t="shared" si="11"/>
+        <v>0.58778525229247292</v>
       </c>
       <c r="H58" s="2">
-        <f t="shared" si="10"/>
-        <v>35200</v>
+        <f t="shared" si="12"/>
+        <v>36044.800000000003</v>
       </c>
       <c r="I58" s="3">
-        <f t="shared" si="4"/>
-        <v>35200</v>
+        <f t="shared" si="6"/>
+        <v>36045</v>
       </c>
       <c r="J58" s="3">
         <f>MOD(I58,$D$6)</f>
-        <v>2432</v>
+        <v>3277</v>
       </c>
       <c r="K58" s="2">
         <f>J58/($D$6)</f>
-        <v>7.421875E-2</v>
+        <v>0.100006103515625</v>
       </c>
       <c r="L58">
-        <f t="shared" si="13"/>
-        <v>2432</v>
+        <f t="shared" si="15"/>
+        <v>3277</v>
       </c>
       <c r="M58" s="2">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
     </row>
@@ -2637,39 +2658,39 @@
         <v>45</v>
       </c>
       <c r="B59" s="6">
-        <f t="shared" si="7"/>
-        <v>4.39453125</v>
+        <f t="shared" si="9"/>
+        <v>4.5</v>
       </c>
       <c r="E59" s="2">
-        <f t="shared" si="8"/>
-        <v>1.0986328125</v>
+        <f t="shared" si="10"/>
+        <v>1.125</v>
       </c>
       <c r="F59" s="8">
-        <f t="shared" si="9"/>
-        <v>0.58081395809576386</v>
+        <f t="shared" si="11"/>
+        <v>0.70710678118654668</v>
       </c>
       <c r="H59" s="2">
-        <f t="shared" si="10"/>
-        <v>36000</v>
+        <f t="shared" si="12"/>
+        <v>36864</v>
       </c>
       <c r="I59" s="3">
-        <f t="shared" si="4"/>
-        <v>36000</v>
+        <f t="shared" si="6"/>
+        <v>36864</v>
       </c>
       <c r="J59" s="3">
         <f>MOD(I59,$D$6)</f>
-        <v>3232</v>
+        <v>4096</v>
       </c>
       <c r="K59" s="2">
         <f>J59/($D$6)</f>
-        <v>9.86328125E-2</v>
+        <v>0.125</v>
       </c>
       <c r="L59">
-        <f t="shared" si="13"/>
-        <v>3232</v>
+        <f t="shared" si="15"/>
+        <v>4096</v>
       </c>
       <c r="M59" s="2">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
     </row>
@@ -2678,39 +2699,39 @@
         <v>46</v>
       </c>
       <c r="B60" s="6">
-        <f t="shared" ref="B60:B61" si="15">A60*1/$C$3*1000</f>
-        <v>4.4921875</v>
+        <f t="shared" ref="B60:B61" si="17">A60*1/$C$3*1000</f>
+        <v>4.5999999999999996</v>
       </c>
       <c r="E60" s="2">
-        <f t="shared" ref="E60:E61" si="16">$C$5*B60/1000</f>
-        <v>1.123046875</v>
+        <f t="shared" ref="E60:E61" si="18">$C$5*B60/1000</f>
+        <v>1.1499999999999999</v>
       </c>
       <c r="F60" s="8">
-        <f t="shared" ref="F60:F61" si="17">SIN(2*PI()*$C$5*B60/1000)</f>
-        <v>0.69837624940897236</v>
+        <f t="shared" ref="F60:F61" si="19">SIN(2*PI()*$C$5*B60/1000)</f>
+        <v>0.80901699437494679</v>
       </c>
       <c r="H60" s="2">
-        <f t="shared" ref="H60:H61" si="18">$J$4*A60</f>
-        <v>36800</v>
+        <f t="shared" ref="H60:H61" si="20">$J$4*A60</f>
+        <v>37683.200000000004</v>
       </c>
       <c r="I60" s="3">
-        <f t="shared" si="4"/>
-        <v>36800</v>
+        <f t="shared" si="6"/>
+        <v>37683</v>
       </c>
       <c r="J60" s="3">
-        <f t="shared" ref="J60:J61" si="19">MOD(I60,$D$6)</f>
-        <v>4032</v>
+        <f t="shared" ref="J60:J61" si="21">MOD(I60,$D$6)</f>
+        <v>4915</v>
       </c>
       <c r="K60" s="2">
-        <f t="shared" ref="K60:K61" si="20">J60/($D$6)</f>
-        <v>0.123046875</v>
+        <f t="shared" ref="K60:K61" si="22">J60/($D$6)</f>
+        <v>0.149993896484375</v>
       </c>
       <c r="L60">
-        <f t="shared" ref="L60:L61" si="21">_xlfn.BITAND(I60,$D$6-1)</f>
-        <v>4032</v>
+        <f t="shared" ref="L60:L61" si="23">_xlfn.BITAND(I60,$D$6-1)</f>
+        <v>4915</v>
       </c>
       <c r="M60" s="2">
-        <f t="shared" ref="M60:M61" si="22">$L$4*B60/1000</f>
+        <f t="shared" ref="M60:M61" si="24">$L$4*B60/1000</f>
         <v>0</v>
       </c>
     </row>
@@ -2719,39 +2740,39 @@
         <v>47</v>
       </c>
       <c r="B61" s="6">
-        <f t="shared" si="15"/>
-        <v>4.58984375</v>
+        <f t="shared" si="17"/>
+        <v>4.7</v>
       </c>
       <c r="E61" s="2">
-        <f t="shared" si="16"/>
-        <v>1.1474609375</v>
+        <f t="shared" si="18"/>
+        <v>1.175</v>
       </c>
       <c r="F61" s="8">
-        <f t="shared" si="17"/>
-        <v>0.79953726910790412</v>
+        <f t="shared" si="19"/>
+        <v>0.89100652418836768</v>
       </c>
       <c r="H61" s="2">
-        <f t="shared" si="18"/>
-        <v>37600</v>
+        <f t="shared" si="20"/>
+        <v>38502.400000000001</v>
       </c>
       <c r="I61" s="3">
-        <f t="shared" si="4"/>
-        <v>37600</v>
+        <f t="shared" si="6"/>
+        <v>38502</v>
       </c>
       <c r="J61" s="3">
-        <f t="shared" si="19"/>
-        <v>4832</v>
+        <f t="shared" si="21"/>
+        <v>5734</v>
       </c>
       <c r="K61" s="2">
-        <f t="shared" si="20"/>
-        <v>0.1474609375</v>
+        <f t="shared" si="22"/>
+        <v>0.17498779296875</v>
       </c>
       <c r="L61">
-        <f t="shared" si="21"/>
-        <v>4832</v>
+        <f t="shared" si="23"/>
+        <v>5734</v>
       </c>
       <c r="M61" s="2">
-        <f t="shared" si="22"/>
+        <f t="shared" si="24"/>
         <v>0</v>
       </c>
     </row>

</xml_diff>